<commit_message>
Caso de prueba 1.1 y 1.2 , borrado backup automatico
</commit_message>
<xml_diff>
--- a/pruebas/Caso_de_prueba_1.2_Identificar Usuario.xlsx
+++ b/pruebas/Caso_de_prueba_1.2_Identificar Usuario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="426" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="212" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Procedimiento de Prueba: </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+  <si>
+    <t>Procedimiento de Prueba: Identificar usuario</t>
   </si>
   <si>
     <t>1- Ingresar a la pantalla de identificación.</t>
@@ -29,6 +29,9 @@
     <t>3- Presionar botón identificarse</t>
   </si>
   <si>
+    <t>Caso de Prueba</t>
+  </si>
+  <si>
     <t>Código</t>
   </si>
   <si>
@@ -47,7 +50,7 @@
     <t>Resultado Obtenido</t>
   </si>
   <si>
-    <t>1.2</t>
+    <t>1.2.1</t>
   </si>
   <si>
     <t>Lograr una identificación correcta
@@ -60,6 +63,52 @@
   <si>
     <t>muestra pantalla principal
 Del sistema</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>Comprobar que se requieran los campos obligatorios</t>
+  </si>
+  <si>
+    <t>usuario:user1
+contraseña:en blanco</t>
+  </si>
+  <si>
+    <t>muestra el aviso en pantalla de que
+Falta contraseña</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>Comprobar que se identifique de manera correcta un 
+Usuario con caracteres especiales</t>
+  </si>
+  <si>
+    <t>usuario:üser1@l0mas
+contraseña:1234</t>
+  </si>
+  <si>
+    <t>1- Ingresar a la pantalla de identificación en dos pestañas o ventanas al mismo tiempo.</t>
+  </si>
+  <si>
+    <t>2- Ingresar Nombre de Usuario y contraseña en cada uno de los formularios</t>
+  </si>
+  <si>
+    <t>3- Presionar botón identificarse en cada uno de los formularios</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>Comprobar que se impida identificar dos veces al 
+Mismo usuario</t>
+  </si>
+  <si>
+    <t>muestra pantalla principal del sistema en la pantalla 1.
+Muestra cartel de error “El usuario ya ha accedido al sistema” en la pantalla 2.
+</t>
   </si>
 </sst>
 </file>
@@ -109,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -124,6 +173,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -150,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,6 +228,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -195,7 +259,7 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -257,53 +321,182 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="12">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>